<commit_message>
Added code to output excel file based on grouping by starhc type and exp type
</commit_message>
<xml_diff>
--- a/output/out_dil+infogest_mir_all_conc_time_True.xlsx
+++ b/output/out_dil+infogest_mir_all_conc_time_True.xlsx
@@ -527,7 +527,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,45 +543,55 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Starch</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Exp_type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Sample_presentation</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Derivative</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Window_length</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Polynomial_order</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>No_of_components</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Score_c</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>RMSEC</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Score_CV</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>RMSECV</t>
         </is>
@@ -598,31 +608,41 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Potato</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>infogest</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>9</v>
-      </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
         <v>0.08878896423328975</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>34.64405450000374</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>-0.0007815514092339715</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>36.3068752632723</v>
       </c>
     </row>
@@ -637,31 +657,41 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>infogest</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>9</v>
-      </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="n">
         <v>0.2220410601622489</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>32.0108764807276</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>-0.0314662703639419</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>36.85927113411959</v>
       </c>
     </row>
@@ -676,32 +706,42 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Pregelled Maize Starch</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>infogest</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>9</v>
-      </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
+        <v>9</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="n">
         <v>3</v>
       </c>
-      <c r="H4" t="n">
-        <v>0.6990113083800298</v>
-      </c>
-      <c r="I4" t="n">
-        <v>20.42734165010175</v>
-      </c>
       <c r="J4" t="n">
-        <v>-0.2083634357097135</v>
+        <v>0.9005916464878736</v>
       </c>
       <c r="K4" t="n">
-        <v>40.92941625706369</v>
+        <v>21.386393677039</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.2676866319066333</v>
+      </c>
+      <c r="M4" t="n">
+        <v>58.04630743292445</v>
       </c>
     </row>
     <row r="5">
@@ -715,32 +755,42 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Gelose 80</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>9</v>
-      </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7573282325799735</v>
+        <v>2</v>
       </c>
       <c r="I5" t="n">
-        <v>18.34198735173641</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
-        <v>0.05829205654498382</v>
+        <v>0.2998025092646853</v>
       </c>
       <c r="K5" t="n">
-        <v>36.13223947199796</v>
+        <v>31.15638329869779</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.158853105476169</v>
+      </c>
+      <c r="M5" t="n">
+        <v>34.14858289665076</v>
       </c>
     </row>
     <row r="6">
@@ -754,32 +804,42 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Gelose 50</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>9</v>
-      </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H6" t="n">
-        <v>0.999745493358435</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5939998332785303</v>
+        <v>3</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.4384273689348221</v>
+        <v>0.6990113083800298</v>
       </c>
       <c r="K6" t="n">
-        <v>44.65609385614521</v>
+        <v>20.42734165010175</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.2083634357097135</v>
+      </c>
+      <c r="M6" t="n">
+        <v>40.92941625706369</v>
       </c>
     </row>
     <row r="7">
@@ -793,32 +853,42 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Potato</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>9</v>
-      </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H7" t="n">
-        <v>0.2998025092646853</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>31.15638329869779</v>
+        <v>7</v>
       </c>
       <c r="J7" t="n">
-        <v>0.158853105476169</v>
+        <v>0.9778464981215428</v>
       </c>
       <c r="K7" t="n">
-        <v>34.14858289665076</v>
+        <v>5.54189070087344</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.5454944036607083</v>
+      </c>
+      <c r="M7" t="n">
+        <v>46.28822010604031</v>
       </c>
     </row>
     <row r="8">
@@ -832,32 +902,42 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>9</v>
-      </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H8" t="n">
-        <v>0.9778464981215428</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>5.54189070087344</v>
+        <v>3</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.5454944036607083</v>
+        <v>0.7573282325799735</v>
       </c>
       <c r="K8" t="n">
-        <v>46.28822010604031</v>
+        <v>18.34198735173641</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.05829205654498382</v>
+      </c>
+      <c r="M8" t="n">
+        <v>36.13223947199796</v>
       </c>
     </row>
     <row r="9">
@@ -871,32 +951,42 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Pregelled Maize Starch</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Turbid</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>9</v>
-      </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>0.9005916464878736</v>
+        <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>21.386393677039</v>
+        <v>11</v>
       </c>
       <c r="J9" t="n">
-        <v>0.2676866319066333</v>
+        <v>0.999745493358435</v>
       </c>
       <c r="K9" t="n">
-        <v>58.04630743292445</v>
+        <v>0.5939998332785303</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-0.4384273689348221</v>
+      </c>
+      <c r="M9" t="n">
+        <v>44.65609385614521</v>
       </c>
     </row>
   </sheetData>
@@ -910,7 +1000,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -926,45 +1016,55 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Starch</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Exp_type</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Sample_presentation</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Derivative</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Window_length</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Polynomial_order</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>No_of_components</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Score_c</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>RMSEC</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Score_CV</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>RMSECV</t>
         </is>
@@ -981,31 +1081,41 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>Potato</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>infogest</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>9</v>
-      </c>
       <c r="F2" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" t="n">
         <v>0.5456312993496129</v>
       </c>
-      <c r="I2" t="n">
+      <c r="K2" t="n">
         <v>24.46377260779245</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>0.03540481874387502</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>35.64443800422116</v>
       </c>
     </row>
@@ -1020,31 +1130,41 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>infogest</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>9</v>
-      </c>
       <c r="F3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" t="n">
+        <v>9</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="n">
         <v>5</v>
       </c>
-      <c r="H3" t="n">
+      <c r="J3" t="n">
         <v>0.8659422329660581</v>
       </c>
-      <c r="I3" t="n">
+      <c r="K3" t="n">
         <v>13.25393150209114</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>0.2651856491506652</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>31.03041228755734</v>
       </c>
     </row>
@@ -1059,32 +1179,42 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>Pregelled Maize Starch</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>infogest</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>9</v>
-      </c>
       <c r="F4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H4" t="n">
-        <v>0.7001866376275945</v>
+        <v>2</v>
       </c>
       <c r="I4" t="n">
-        <v>20.38741932636373</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.3185225568487282</v>
+        <v>0.3257163204922318</v>
       </c>
       <c r="K4" t="n">
-        <v>42.75437331489722</v>
+        <v>56.94995594337954</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.03180849867308788</v>
+      </c>
+      <c r="M4" t="n">
+        <v>68.24215007272944</v>
       </c>
     </row>
     <row r="5">
@@ -1098,32 +1228,42 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Gelose 80</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>9</v>
-      </c>
       <c r="F5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2407393586860641</v>
+        <v>2</v>
       </c>
       <c r="I5" t="n">
-        <v>32.44383669662218</v>
+        <v>2</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.6282783746602121</v>
+        <v>0.7020585222288871</v>
       </c>
       <c r="K5" t="n">
-        <v>47.51175694212198</v>
+        <v>20.32367525207522</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-0.3281005412441858</v>
+      </c>
+      <c r="M5" t="n">
+        <v>42.90938004403169</v>
       </c>
     </row>
     <row r="6">
@@ -1137,32 +1277,42 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Gelose 50</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>9</v>
-      </c>
       <c r="F6" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H6" t="n">
-        <v>0.5866761369756864</v>
+        <v>2</v>
       </c>
       <c r="I6" t="n">
-        <v>23.93767701807853</v>
+        <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.2762485691660697</v>
+        <v>0.7001866376275945</v>
       </c>
       <c r="K6" t="n">
-        <v>42.06340224532839</v>
+        <v>20.38741932636373</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-0.3185225568487282</v>
+      </c>
+      <c r="M6" t="n">
+        <v>42.75437331489722</v>
       </c>
     </row>
     <row r="7">
@@ -1176,32 +1326,42 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>Potato</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="n">
-        <v>9</v>
-      </c>
       <c r="F7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G7" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H7" t="n">
-        <v>0.7020585222288871</v>
+        <v>2</v>
       </c>
       <c r="I7" t="n">
-        <v>20.32367525207522</v>
+        <v>2</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.3281005412441858</v>
+        <v>0.8137302007733409</v>
       </c>
       <c r="K7" t="n">
-        <v>42.90938004403169</v>
+        <v>16.06970803407225</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-0.8557782255894217</v>
+      </c>
+      <c r="M7" t="n">
+        <v>50.72240067611544</v>
       </c>
     </row>
     <row r="8">
@@ -1215,32 +1375,42 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>Rice</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="n">
-        <v>9</v>
-      </c>
       <c r="F8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G8" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="H8" t="n">
-        <v>0.8137302007733409</v>
+        <v>2</v>
       </c>
       <c r="I8" t="n">
-        <v>16.06970803407225</v>
+        <v>1</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.8557782255894217</v>
+        <v>0.2407393586860641</v>
       </c>
       <c r="K8" t="n">
-        <v>50.72240067611544</v>
+        <v>32.44383669662218</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-0.6282783746602121</v>
+      </c>
+      <c r="M8" t="n">
+        <v>47.51175694212198</v>
       </c>
     </row>
     <row r="9">
@@ -1254,32 +1424,42 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>Pregelled Maize Starch</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>dil</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Supernatant</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>9</v>
-      </c>
       <c r="F9" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="H9" t="n">
-        <v>0.3257163204922318</v>
+        <v>2</v>
       </c>
       <c r="I9" t="n">
-        <v>56.94995594337954</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>0.03180849867308788</v>
+        <v>0.5866761369756864</v>
       </c>
       <c r="K9" t="n">
-        <v>68.24215007272944</v>
+        <v>23.93767701807853</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-0.2762485691660697</v>
+      </c>
+      <c r="M9" t="n">
+        <v>42.06340224532839</v>
       </c>
     </row>
   </sheetData>

</xml_diff>